<commit_message>
SMTP Attachment integreted with pdf
</commit_message>
<xml_diff>
--- a/Output/CandidateExtracted.xlsx
+++ b/Output/CandidateExtracted.xlsx
@@ -34,28 +34,28 @@
     <x:t>Back-End</x:t>
   </x:si>
   <x:si>
+    <x:t>8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Iacopo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>De Palatis</x:t>
+  </x:si>
+  <x:si>
+    <x:t>25</x:t>
+  </x:si>
+  <x:si>
+    <x:t>iacopo@gmail.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3232854389</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Full-Stack</x:t>
+  </x:si>
+  <x:si>
     <x:t>10</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Simona</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Laurenzi</x:t>
-  </x:si>
-  <x:si>
-    <x:t>29</x:t>
-  </x:si>
-  <x:si>
-    <x:t>simona@yahoo.it</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3239569455</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Front-End</x:t>
-  </x:si>
-  <x:si>
-    <x:t>8</x:t>
   </x:si>
 </x:sst>
 </file>

</xml_diff>